<commit_message>
this is my cart page
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/opencartTestData.xlsx
+++ b/src/test/resources/testdata/opencartTestData.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Eclipse-Selenium Practice\POMSeries\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC142BB-C281-40D3-A080-25903EFD999B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CBF79C8-D092-477F-BAC9-28EE43C2A20B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="36" windowWidth="17280" windowHeight="12468" xr2:uid="{87D8F335-19F8-44EB-8905-896E3A1693FC}"/>
+    <workbookView xWindow="11244" yWindow="192" windowWidth="17280" windowHeight="12468" xr2:uid="{87D8F335-19F8-44EB-8905-896E3A1693FC}"/>
   </bookViews>
   <sheets>
-    <sheet name="register " sheetId="1" r:id="rId1"/>
+    <sheet name="register" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -491,7 +491,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>